<commit_message>
push ulang setelah diremoved
</commit_message>
<xml_diff>
--- a/minggu-1/02/latihan2ContohCRCcard.xlsx
+++ b/minggu-1/02/latihan2ContohCRCcard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\praxis-academy\minggu-1\02\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A61C0D70-996C-4E28-911F-DB7D8B8FE095}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{80798C5B-4E11-43CC-A004-384C89402CA1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{67229D71-84C5-4BFB-8EC4-0B8899EBB84F}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="16">
   <si>
     <t>Class</t>
   </si>
@@ -298,52 +298,52 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -843,35 +843,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="9"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="6"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="11"/>
+      <c r="B2" s="8"/>
       <c r="C2" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="13"/>
+      <c r="B3" s="19"/>
       <c r="C3" s="3" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="6"/>
+      <c r="B4" s="10"/>
       <c r="C4" s="2" t="s">
         <v>13</v>
       </c>
@@ -880,98 +880,92 @@
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E5" s="14" t="s">
+      <c r="E5" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="15"/>
-      <c r="G5" s="16"/>
-      <c r="J5" s="19" t="s">
+      <c r="F5" s="12"/>
+      <c r="G5" s="13"/>
+      <c r="J5" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="K5" s="8"/>
-      <c r="L5" s="9"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="6"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="17"/>
+      <c r="F6" s="14"/>
       <c r="G6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J6" s="10" t="s">
+      <c r="J6" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="K6" s="11"/>
+      <c r="K6" s="8"/>
       <c r="L6" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="18"/>
+      <c r="F7" s="16"/>
       <c r="G7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="J7" s="4" t="s">
+      <c r="J7" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="K7" s="6"/>
+      <c r="K7" s="10"/>
       <c r="L7" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="5"/>
+      <c r="F8" s="17"/>
       <c r="G8" s="2"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="15"/>
-      <c r="C10" s="16"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="13"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="17"/>
+      <c r="B11" s="14"/>
       <c r="C11" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="12" t="s">
+      <c r="A12" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="18"/>
+      <c r="B12" s="16"/>
       <c r="C12" s="3" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="5"/>
+      <c r="B13" s="17"/>
       <c r="C13" s="2" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="J5:L5"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="E8:F8"/>
     <mergeCell ref="A4:B4"/>
@@ -981,6 +975,12 @@
     <mergeCell ref="A10:C10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
+    <mergeCell ref="J5:L5"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>